<commit_message>
ClinVar Data added, viz updates
</commit_message>
<xml_diff>
--- a/Data/SNV_filtering_inputs/PillarProject_filtering/BARD1/20250827_BARD1_filter_entry.xlsx
+++ b/Data/SNV_filtering_inputs/PillarProject_filtering/BARD1/20250827_BARD1_filter_entry.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ivan/Documents/GitHub/BARD1_SGE_analysis/Data/SNV_filtering_inputs/PillarProject_filtering/BARD1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F6DCED-28C1-1D44-88CD-68DFFB16C1B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECB78DFA-7576-6D48-8AA9-3EED8A7D7543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="targets" sheetId="1" r:id="rId1"/>
@@ -1026,7 +1026,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1044,10 +1044,10 @@
     </row>
     <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
+        <v>214725146</v>
+      </c>
+      <c r="B2" s="2">
         <v>214810183</v>
-      </c>
-      <c r="B2" s="2">
-        <v>214725146</v>
       </c>
       <c r="C2">
         <v>0</v>

</xml_diff>